<commit_message>
Stakeholder verbessert, Folien ergänzt
</commit_message>
<xml_diff>
--- a/Stakeholderanalyse.xlsx
+++ b/Stakeholderanalyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files (x86)\EPWS2223HausenKochZimmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5B458C-21B0-4121-9C9A-F8BFAADAEDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8D36D3-D15A-4EEC-B513-50F450556432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{1EC1A410-8258-43E6-AE3C-02DE8233B07A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EC1A410-8258-43E6-AE3C-02DE8233B07A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Anforderungsermittlung & Stakeholderanalyse
Anforderungsermittlung überarbeitet und 2 neue Stakeholder hinzugefügt
</commit_message>
<xml_diff>
--- a/Stakeholderanalyse.xlsx
+++ b/Stakeholderanalyse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files (x86)\EPWS2223HausenKochZimmer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederik\Documents\GitHub\EPWS2223HausenKochZimmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D655E0-E552-41A3-8E13-E6E1E2D1B0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A1C310-0A9E-4E67-BBDE-8B29E07983CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EC1A410-8258-43E6-AE3C-02DE8233B07A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EC1A410-8258-43E6-AE3C-02DE8233B07A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Bezeichnung (E/O)</t>
   </si>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>Role angezeit wird</t>
+  </si>
+  <si>
+    <t>Digitale Archive</t>
+  </si>
+  <si>
+    <t>Interesse</t>
+  </si>
+  <si>
+    <t>Inhalte</t>
+  </si>
+  <si>
+    <t>Zur erhöhten Recherchierbarkeit besteht ein Interesse das System und dessen Inhalte mit digitalen Archiven und deren Inhalte zu vernetzen.</t>
+  </si>
+  <si>
+    <t>Staat Deutschland</t>
+  </si>
+  <si>
+    <t>Der deutsche Staat hat den Anspruch, dass das System nicht gegen deutsches Recht verstößt.</t>
   </si>
 </sst>
 </file>
@@ -265,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,8 +314,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -580,19 +604,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -633,51 +740,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,7 +826,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -989,13 +1122,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0898466-D973-4392-B5CB-258D34DDA08A}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -1006,364 +1139,364 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="5" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="5" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="5" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="5" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="32" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="32" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="16" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="6" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="5" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="18" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40"/>
-      <c r="C16" s="20" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="39"/>
+      <c r="E16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="22" t="s">
+      <c r="B18" s="33"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="23"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="22" t="s">
+      <c r="B19" s="33"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="23"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="32" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="22" t="s">
+      <c r="D20" s="36"/>
+      <c r="E20" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="23"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="5" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="34"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="18" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="5" t="s">
+      <c r="B24" s="33"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="34"/>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="5" t="s">
+      <c r="D25" s="36"/>
+      <c r="E25" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="5" t="s">
+      <c r="B26" s="33"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="5" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="5" t="s">
+      <c r="A29" s="30"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="6" t="s">
+      <c r="A30" s="30"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="23" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="37"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="36"/>
       <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="34"/>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="33"/>
+      <c r="C34" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="7" t="s">
+      <c r="D34" s="39"/>
+      <c r="E34" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1371,53 +1504,67 @@
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="12"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="12"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="12"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="12"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
+      <c r="B39" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="45" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D16"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D34"/>
     <mergeCell ref="A27:A30"/>
@@ -1431,6 +1578,17 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>